<commit_message>
Add the screenshot function.
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -1,38 +1,405 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView windowWidth="28695" windowHeight="13335"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Crash Detail" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="144525"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6">
+  <si>
+    <t>Crash</t>
+  </si>
+  <si>
+    <t>Time</t>
+  </si>
+  <si>
+    <t>Seed</t>
+  </si>
+  <si>
+    <t>Test</t>
+  </si>
+  <si>
+    <t>2018-01-26-19:28:47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">:Monkey: seed=1517187665177 count=200
+</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+  <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -40,18 +407,329 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="50">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="8" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="29" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="2">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+  <cellStyles count="50">
+    <cellStyle name="常规" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="1"/>
+    <cellStyle name="60% - 强调文字颜色 6" xfId="2" builtinId="52"/>
+    <cellStyle name="20% - 强调文字颜色 4" xfId="3" builtinId="42"/>
+    <cellStyle name="强调文字颜色 4" xfId="4" builtinId="41"/>
+    <cellStyle name="输入" xfId="5" builtinId="20"/>
+    <cellStyle name="40% - 强调文字颜色 3" xfId="6" builtinId="39"/>
+    <cellStyle name="20% - 强调文字颜色 3" xfId="7" builtinId="38"/>
+    <cellStyle name="货币" xfId="8" builtinId="4"/>
+    <cellStyle name="强调文字颜色 3" xfId="9" builtinId="37"/>
+    <cellStyle name="百分比" xfId="10" builtinId="5"/>
+    <cellStyle name="60% - 强调文字颜色 2" xfId="11" builtinId="36"/>
+    <cellStyle name="60% - 强调文字颜色 5" xfId="12" builtinId="48"/>
+    <cellStyle name="强调文字颜色 2" xfId="13" builtinId="33"/>
+    <cellStyle name="60% - 强调文字颜色 1" xfId="14" builtinId="32"/>
+    <cellStyle name="60% - 强调文字颜色 4" xfId="15" builtinId="44"/>
+    <cellStyle name="计算" xfId="16" builtinId="22"/>
+    <cellStyle name="强调文字颜色 1" xfId="17" builtinId="29"/>
+    <cellStyle name="适中" xfId="18" builtinId="28"/>
+    <cellStyle name="20% - 强调文字颜色 5" xfId="19" builtinId="46"/>
+    <cellStyle name="好" xfId="20" builtinId="26"/>
+    <cellStyle name="20% - 强调文字颜色 1" xfId="21" builtinId="30"/>
+    <cellStyle name="汇总" xfId="22" builtinId="25"/>
+    <cellStyle name="差" xfId="23" builtinId="27"/>
+    <cellStyle name="检查单元格" xfId="24" builtinId="23"/>
+    <cellStyle name="输出" xfId="25" builtinId="21"/>
+    <cellStyle name="标题 1" xfId="26" builtinId="16"/>
+    <cellStyle name="解释性文本" xfId="27" builtinId="53"/>
+    <cellStyle name="20% - 强调文字颜色 2" xfId="28" builtinId="34"/>
+    <cellStyle name="标题 4" xfId="29" builtinId="19"/>
+    <cellStyle name="货币[0]" xfId="30" builtinId="7"/>
+    <cellStyle name="40% - 强调文字颜色 4" xfId="31" builtinId="43"/>
+    <cellStyle name="千位分隔" xfId="32" builtinId="3"/>
+    <cellStyle name="已访问的超链接" xfId="33" builtinId="9"/>
+    <cellStyle name="标题" xfId="34" builtinId="15"/>
+    <cellStyle name="40% - 强调文字颜色 2" xfId="35" builtinId="35"/>
+    <cellStyle name="警告文本" xfId="36" builtinId="11"/>
+    <cellStyle name="60% - 强调文字颜色 3" xfId="37" builtinId="40"/>
+    <cellStyle name="注释" xfId="38" builtinId="10"/>
+    <cellStyle name="20% - 强调文字颜色 6" xfId="39" builtinId="50"/>
+    <cellStyle name="强调文字颜色 5" xfId="40" builtinId="45"/>
+    <cellStyle name="40% - 强调文字颜色 6" xfId="41" builtinId="51"/>
+    <cellStyle name="超链接" xfId="42" builtinId="8"/>
+    <cellStyle name="千位分隔[0]" xfId="43" builtinId="6"/>
+    <cellStyle name="标题 2" xfId="44" builtinId="17"/>
+    <cellStyle name="40% - 强调文字颜色 5" xfId="45" builtinId="47"/>
+    <cellStyle name="标题 3" xfId="46" builtinId="18"/>
+    <cellStyle name="强调文字颜色 6" xfId="47" builtinId="49"/>
+    <cellStyle name="40% - 强调文字颜色 1" xfId="48" builtinId="31"/>
+    <cellStyle name="链接单元格" xfId="49" builtinId="24"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
 </file>
 
@@ -60,7 +738,7 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText" lastClr="313739"/>
       </a:dk1>
       <a:lt1>
         <a:sysClr val="window" lastClr="FFFFFF"/>
@@ -339,13 +1017,45 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr/>
+  <dimension ref="A1:C2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="28.1583333333333" customWidth="1"/>
+    <col min="2" max="2" width="30.125" customWidth="1"/>
+    <col min="3" max="3" width="41.9416666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.699305555555556" right="0.699305555555556" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix the README.md file.
</commit_message>
<xml_diff>
--- a/report.xlsx
+++ b/report.xlsx
@@ -40,10 +40,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="21">
     <font>
@@ -54,10 +54,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="134"/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -83,6 +83,13 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -99,61 +106,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -167,8 +122,45 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -182,24 +174,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
       <color theme="1"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -214,187 +214,187 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -426,8 +426,47 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -456,21 +495,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -488,15 +512,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -505,169 +520,154 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="50">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="17" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="13" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1022,12 +1022,14 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.25" outlineLevelRow="1" outlineLevelCol="2"/>
   <cols>
     <col min="2" max="2" width="54.7333333333333" customWidth="1"/>
+    <col min="3" max="3" width="48.125" customWidth="1"/>
+    <col min="4" max="4" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">

</xml_diff>